<commit_message>
planilha de 2000 iteracoes do fss.
</commit_message>
<xml_diff>
--- a/src/produtos/dataset/ECCOLI/Execucoes_MLP_FSS(RENATO).xlsx
+++ b/src/produtos/dataset/ECCOLI/Execucoes_MLP_FSS(RENATO).xlsx
@@ -1,24 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27224"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eduardo\workspace\br.ufpe.cin.mlp.fss.pso\src\produtos\dataset\ECCOLI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/moura/Pessoal/mestrado/br.ufpe.cin.mlp.fss.pso/src/produtos/dataset/ECCOLI/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="6090" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25180" windowHeight="15460" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ITERACOES 100" sheetId="3" r:id="rId1"/>
     <sheet name="ITERACOES 500" sheetId="5" r:id="rId2"/>
     <sheet name="ITERACOES 1000" sheetId="4" r:id="rId3"/>
+    <sheet name="ITERACOES 2000" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -26,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="10">
   <si>
     <t>tempo médio</t>
   </si>
@@ -54,12 +61,15 @@
   <si>
     <t>1000 iterações</t>
   </si>
+  <si>
+    <t>2000 iterações</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -83,6 +93,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -101,8 +127,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -125,7 +153,9 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -406,60 +436,60 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="160" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
       <selection activeCell="G9" sqref="G9:G40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="19.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="4"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="4"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="4"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="4"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B5" s="4"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="4"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="4"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>2</v>
       </c>
@@ -483,7 +513,7 @@
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
@@ -501,7 +531,7 @@
       </c>
       <c r="I10" s="6"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2</v>
       </c>
@@ -519,7 +549,7 @@
       </c>
       <c r="I11" s="6"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>3</v>
       </c>
@@ -537,7 +567,7 @@
       </c>
       <c r="I12" s="6"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>4</v>
       </c>
@@ -555,7 +585,7 @@
       </c>
       <c r="I13" s="6"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>5</v>
       </c>
@@ -573,7 +603,7 @@
       </c>
       <c r="I14" s="6"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>6</v>
       </c>
@@ -591,7 +621,7 @@
       </c>
       <c r="I15" s="6"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>7</v>
       </c>
@@ -609,7 +639,7 @@
       </c>
       <c r="I16" s="6"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>8</v>
       </c>
@@ -627,7 +657,7 @@
       </c>
       <c r="I17" s="6"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>9</v>
       </c>
@@ -645,7 +675,7 @@
       </c>
       <c r="I18" s="6"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>10</v>
       </c>
@@ -663,7 +693,7 @@
       </c>
       <c r="I19" s="6"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>11</v>
       </c>
@@ -681,7 +711,7 @@
       </c>
       <c r="I20" s="6"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>12</v>
       </c>
@@ -699,7 +729,7 @@
       </c>
       <c r="I21" s="6"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>13</v>
       </c>
@@ -717,7 +747,7 @@
       </c>
       <c r="I22" s="6"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>14</v>
       </c>
@@ -735,7 +765,7 @@
       </c>
       <c r="I23" s="6"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>15</v>
       </c>
@@ -753,7 +783,7 @@
       </c>
       <c r="I24" s="6"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>16</v>
       </c>
@@ -771,7 +801,7 @@
       </c>
       <c r="I25" s="6"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>17</v>
       </c>
@@ -789,7 +819,7 @@
       </c>
       <c r="I26" s="6"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>18</v>
       </c>
@@ -807,7 +837,7 @@
       </c>
       <c r="I27" s="6"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>19</v>
       </c>
@@ -825,7 +855,7 @@
       </c>
       <c r="I28" s="6"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>20</v>
       </c>
@@ -843,7 +873,7 @@
       </c>
       <c r="I29" s="6"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>21</v>
       </c>
@@ -861,7 +891,7 @@
       </c>
       <c r="I30" s="6"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>22</v>
       </c>
@@ -879,7 +909,7 @@
       </c>
       <c r="I31" s="6"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>23</v>
       </c>
@@ -897,7 +927,7 @@
       </c>
       <c r="I32" s="6"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>24</v>
       </c>
@@ -915,7 +945,7 @@
       </c>
       <c r="I33" s="6"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>25</v>
       </c>
@@ -933,7 +963,7 @@
       </c>
       <c r="I34" s="6"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>26</v>
       </c>
@@ -951,7 +981,7 @@
       </c>
       <c r="I35" s="6"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>27</v>
       </c>
@@ -969,7 +999,7 @@
       </c>
       <c r="I36" s="6"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>28</v>
       </c>
@@ -987,7 +1017,7 @@
       </c>
       <c r="I37" s="6"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>29</v>
       </c>
@@ -1005,7 +1035,7 @@
       </c>
       <c r="I38" s="6"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>30</v>
       </c>
@@ -1023,7 +1053,7 @@
       </c>
       <c r="I39" s="6"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>0</v>
       </c>
@@ -1053,13 +1083,13 @@
       <selection sqref="A1:E40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
@@ -1068,7 +1098,7 @@
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>6</v>
       </c>
@@ -1077,7 +1107,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>5</v>
       </c>
@@ -1086,7 +1116,7 @@
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>7</v>
       </c>
@@ -1095,35 +1125,35 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="7"/>
       <c r="B5" s="10"/>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="8"/>
       <c r="B6" s="10"/>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="8"/>
       <c r="B7" s="10"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="8"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="24" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>2</v>
       </c>
@@ -1140,7 +1170,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="7">
         <v>1</v>
       </c>
@@ -1157,7 +1187,7 @@
         <v>0.45793576392505397</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="7">
         <v>2</v>
       </c>
@@ -1174,7 +1204,7 @@
         <v>0.46297657505803402</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="7">
         <v>3</v>
       </c>
@@ -1191,7 +1221,7 @@
         <v>0.47868364883617698</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="7">
         <v>4</v>
       </c>
@@ -1208,7 +1238,7 @@
         <v>0.47613169339600298</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="7">
         <v>5</v>
       </c>
@@ -1225,7 +1255,7 @@
         <v>0.48153642901525701</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="7">
         <v>6</v>
       </c>
@@ -1242,7 +1272,7 @@
         <v>0.48457371413939199</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="7">
         <v>7</v>
       </c>
@@ -1259,7 +1289,7 @@
         <v>0.48883562045064</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="7">
         <v>8</v>
       </c>
@@ -1276,7 +1306,7 @@
         <v>0.48470122293395601</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="7">
         <v>9</v>
       </c>
@@ -1293,7 +1323,7 @@
         <v>0.48385285398892502</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="7">
         <v>10</v>
       </c>
@@ -1310,7 +1340,7 @@
         <v>0.48332089147228402</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="7">
         <v>11</v>
       </c>
@@ -1327,7 +1357,7 @@
         <v>0.48343121473936501</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="7">
         <v>12</v>
       </c>
@@ -1344,7 +1374,7 @@
         <v>0.48144535867905902</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="7">
         <v>13</v>
       </c>
@@ -1361,7 +1391,7 @@
         <v>0.48085570147448797</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="7">
         <v>14</v>
       </c>
@@ -1378,7 +1408,7 @@
         <v>0.48391730875578598</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="7">
         <v>15</v>
       </c>
@@ -1395,7 +1425,7 @@
         <v>0.48312507369869001</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="7">
         <v>16</v>
       </c>
@@ -1412,7 +1442,7 @@
         <v>0.48309211892188803</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="7">
         <v>17</v>
       </c>
@@ -1429,7 +1459,7 @@
         <v>0.48181238784654001</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="7">
         <v>18</v>
       </c>
@@ -1446,7 +1476,7 @@
         <v>0.48098406125406901</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="7">
         <v>19</v>
       </c>
@@ -1463,7 +1493,7 @@
         <v>0.47834724457029298</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="7">
         <v>20</v>
       </c>
@@ -1480,7 +1510,7 @@
         <v>0.47808221238987603</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="7">
         <v>21</v>
       </c>
@@ -1497,7 +1527,7 @@
         <v>0.47882360354562398</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="7">
         <v>22</v>
       </c>
@@ -1514,7 +1544,7 @@
         <v>0.476916958058267</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="7">
         <v>23</v>
       </c>
@@ -1531,7 +1561,7 @@
         <v>0.47493637958540003</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="7">
         <v>24</v>
       </c>
@@ -1548,7 +1578,7 @@
         <v>0.47322581256533403</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="7">
         <v>25</v>
       </c>
@@ -1565,7 +1595,7 @@
         <v>0.47330114100759502</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="7">
         <v>26</v>
       </c>
@@ -1582,7 +1612,7 @@
         <v>0.47314102945271203</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="7">
         <v>27</v>
       </c>
@@ -1599,7 +1629,7 @@
         <v>0.472736173472043</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="7">
         <v>28</v>
       </c>
@@ -1616,7 +1646,7 @@
         <v>0.47238832617542498</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="7">
         <v>29</v>
       </c>
@@ -1633,7 +1663,7 @@
         <v>0.47247061776113503</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="7">
         <v>30</v>
       </c>
@@ -1650,7 +1680,7 @@
         <v>0.47234172834787902</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
         <v>0</v>
       </c>
@@ -1676,17 +1706,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection sqref="A1:E40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
@@ -1695,7 +1725,7 @@
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>4</v>
       </c>
@@ -1704,7 +1734,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>5</v>
       </c>
@@ -1713,7 +1743,7 @@
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>8</v>
       </c>
@@ -1722,35 +1752,35 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="7"/>
       <c r="B5" s="10"/>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="8"/>
       <c r="B6" s="10"/>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="8"/>
       <c r="B7" s="10"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="8"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="24" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>2</v>
       </c>
@@ -1767,7 +1797,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="7">
         <v>1</v>
       </c>
@@ -1784,7 +1814,7 @@
         <v>0.43590921828176299</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="7">
         <v>2</v>
       </c>
@@ -1801,7 +1831,7 @@
         <v>0.47471104658067098</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="7">
         <v>3</v>
       </c>
@@ -1818,7 +1848,7 @@
         <v>0.473494135361618</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="7">
         <v>4</v>
       </c>
@@ -1835,7 +1865,7 @@
         <v>0.47862708439600898</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="7">
         <v>5</v>
       </c>
@@ -1852,7 +1882,7 @@
         <v>0.47984609647911602</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="7">
         <v>6</v>
       </c>
@@ -1869,7 +1899,7 @@
         <v>0.48095061242906001</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="7">
         <v>7</v>
       </c>
@@ -1886,7 +1916,7 @@
         <v>0.48407199270583101</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="7">
         <v>8</v>
       </c>
@@ -1903,7 +1933,7 @@
         <v>0.48559874321353502</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="7">
         <v>9</v>
       </c>
@@ -1920,7 +1950,7 @@
         <v>0.48586810525965801</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="7">
         <v>10</v>
       </c>
@@ -1937,7 +1967,7 @@
         <v>0.48602042341061003</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="7">
         <v>11</v>
       </c>
@@ -1954,7 +1984,7 @@
         <v>0.48515116522338803</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="7">
         <v>12</v>
       </c>
@@ -1971,7 +2001,7 @@
         <v>0.48363565795059499</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="7">
         <v>13</v>
       </c>
@@ -1988,7 +2018,7 @@
         <v>0.48248773600503903</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="7">
         <v>14</v>
       </c>
@@ -2005,7 +2035,7 @@
         <v>0.47983409231339602</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="7">
         <v>15</v>
       </c>
@@ -2022,7 +2052,7 @@
         <v>0.478132259417481</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="7">
         <v>16</v>
       </c>
@@ -2039,7 +2069,7 @@
         <v>0.47901097996464898</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="7">
         <v>17</v>
       </c>
@@ -2056,7 +2086,7 @@
         <v>0.48059566845491702</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="7">
         <v>18</v>
       </c>
@@ -2073,7 +2103,7 @@
         <v>0.48197852862116602</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="7">
         <v>19</v>
       </c>
@@ -2090,7 +2120,7 @@
         <v>0.48389011495468998</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="7">
         <v>20</v>
       </c>
@@ -2107,7 +2137,7 @@
         <v>0.48471388380236302</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="7">
         <v>21</v>
       </c>
@@ -2124,7 +2154,7 @@
         <v>0.484231653487671</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="7">
         <v>22</v>
       </c>
@@ -2141,7 +2171,7 @@
         <v>0.48424914527622698</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="7">
         <v>23</v>
       </c>
@@ -2158,7 +2188,7 @@
         <v>0.48447895882918302</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="7">
         <v>24</v>
       </c>
@@ -2175,7 +2205,7 @@
         <v>0.48567891554584403</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="7">
         <v>25</v>
       </c>
@@ -2192,7 +2222,7 @@
         <v>0.48563871317955698</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="7">
         <v>26</v>
       </c>
@@ -2209,7 +2239,7 @@
         <v>0.48574017706511302</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="7">
         <v>27</v>
       </c>
@@ -2226,7 +2256,7 @@
         <v>0.486286254570646</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="7">
         <v>28</v>
       </c>
@@ -2243,7 +2273,7 @@
         <v>0.48655124907008401</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="7">
         <v>29</v>
       </c>
@@ -2260,7 +2290,7 @@
         <v>0.48775575764642198</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="7">
         <v>30</v>
       </c>
@@ -2277,7 +2307,7 @@
         <v>0.48819785004903099</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
         <v>0</v>
       </c>
@@ -2296,5 +2326,632 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="35" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="10"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="10"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="10"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="7"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="8"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="8"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="8"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+    </row>
+    <row r="9" spans="1:5" ht="24" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="10">
+        <v>10</v>
+      </c>
+      <c r="C9" s="10">
+        <v>20</v>
+      </c>
+      <c r="D9" s="10">
+        <v>50</v>
+      </c>
+      <c r="E9" s="10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="7">
+        <v>1</v>
+      </c>
+      <c r="B10" s="7">
+        <v>0.442496084537356</v>
+      </c>
+      <c r="C10" s="7">
+        <v>0.356542546615636</v>
+      </c>
+      <c r="D10">
+        <v>0.41978974555784898</v>
+      </c>
+      <c r="E10" s="7">
+        <v>0.59193112215383203</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="7">
+        <v>2</v>
+      </c>
+      <c r="B11" s="7">
+        <v>0.43086871113966801</v>
+      </c>
+      <c r="C11" s="7">
+        <v>0.42956881749951598</v>
+      </c>
+      <c r="D11">
+        <v>0.422502271960499</v>
+      </c>
+      <c r="E11" s="7">
+        <v>0.50518965934307303</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="7">
+        <v>3</v>
+      </c>
+      <c r="B12" s="7">
+        <v>0.415997502782329</v>
+      </c>
+      <c r="C12" s="7">
+        <v>0.43409864389493802</v>
+      </c>
+      <c r="D12">
+        <v>0.44172138289287599</v>
+      </c>
+      <c r="E12" s="7">
+        <v>0.50050155177436795</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="7">
+        <v>4</v>
+      </c>
+      <c r="B13" s="7">
+        <v>0.4075272468958</v>
+      </c>
+      <c r="C13" s="7">
+        <v>0.43501254349705698</v>
+      </c>
+      <c r="D13">
+        <v>0.44424541467573803</v>
+      </c>
+      <c r="E13" s="7">
+        <v>0.49650075441082298</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="7">
+        <v>5</v>
+      </c>
+      <c r="B14" s="7">
+        <v>0.41756590683755301</v>
+      </c>
+      <c r="C14" s="7">
+        <v>0.42652647000835903</v>
+      </c>
+      <c r="D14">
+        <v>0.45241504807212901</v>
+      </c>
+      <c r="E14" s="7">
+        <v>0.49457315828410198</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="7">
+        <v>6</v>
+      </c>
+      <c r="B15" s="7">
+        <v>0.41858404718127701</v>
+      </c>
+      <c r="C15" s="7">
+        <v>0.42806980673726902</v>
+      </c>
+      <c r="D15">
+        <v>0.45715753747021898</v>
+      </c>
+      <c r="E15" s="7">
+        <v>0.49067558730829702</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="7">
+        <v>7</v>
+      </c>
+      <c r="B16" s="7">
+        <v>0.41712659420536502</v>
+      </c>
+      <c r="C16" s="7">
+        <v>0.43039761873034799</v>
+      </c>
+      <c r="D16">
+        <v>0.460998246260163</v>
+      </c>
+      <c r="E16" s="7">
+        <v>0.49261714149757602</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="7">
+        <v>8</v>
+      </c>
+      <c r="B17" s="7">
+        <v>0.41165725472041598</v>
+      </c>
+      <c r="C17" s="7">
+        <v>0.43494654147317402</v>
+      </c>
+      <c r="D17">
+        <v>0.46542657696082701</v>
+      </c>
+      <c r="E17" s="7">
+        <v>0.49526489718225403</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="7">
+        <v>9</v>
+      </c>
+      <c r="B18" s="7">
+        <v>0.41382105990315698</v>
+      </c>
+      <c r="C18" s="7">
+        <v>0.44104029266287897</v>
+      </c>
+      <c r="D18">
+        <v>0.46498828213769899</v>
+      </c>
+      <c r="E18" s="7">
+        <v>0.49076969474724103</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="7">
+        <v>10</v>
+      </c>
+      <c r="B19" s="7">
+        <v>0.41591321216376897</v>
+      </c>
+      <c r="C19" s="7">
+        <v>0.44417045263841798</v>
+      </c>
+      <c r="D19">
+        <v>0.46535283076218398</v>
+      </c>
+      <c r="E19" s="7">
+        <v>0.49305166146585599</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="7">
+        <v>11</v>
+      </c>
+      <c r="B20" s="7">
+        <v>0.42049371198825503</v>
+      </c>
+      <c r="C20" s="7">
+        <v>0.44569323298236402</v>
+      </c>
+      <c r="D20">
+        <v>0.46669218346089603</v>
+      </c>
+      <c r="E20" s="7">
+        <v>0.49604504729885401</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="7">
+        <v>12</v>
+      </c>
+      <c r="B21" s="7">
+        <v>0.42070268068577299</v>
+      </c>
+      <c r="C21" s="7">
+        <v>0.446651136427138</v>
+      </c>
+      <c r="D21">
+        <v>0.463241733953281</v>
+      </c>
+      <c r="E21" s="7">
+        <v>0.49558805103791198</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="7">
+        <v>13</v>
+      </c>
+      <c r="B22" s="7">
+        <v>0.42198934465319898</v>
+      </c>
+      <c r="C22" s="7">
+        <v>0.447908045723589</v>
+      </c>
+      <c r="D22">
+        <v>0.46606882685753098</v>
+      </c>
+      <c r="E22" s="7">
+        <v>0.49410009911707198</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="7">
+        <v>14</v>
+      </c>
+      <c r="B23" s="7">
+        <v>0.42404327417778698</v>
+      </c>
+      <c r="C23" s="7">
+        <v>0.44566897636008801</v>
+      </c>
+      <c r="D23">
+        <v>0.46476799228559101</v>
+      </c>
+      <c r="E23" s="7">
+        <v>0.49867633241752801</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="7">
+        <v>15</v>
+      </c>
+      <c r="B24" s="7">
+        <v>0.427648435083678</v>
+      </c>
+      <c r="C24" s="7">
+        <v>0.451009137401918</v>
+      </c>
+      <c r="D24">
+        <v>0.46748873490668902</v>
+      </c>
+      <c r="E24" s="7">
+        <v>0.49899940824634198</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="7">
+        <v>16</v>
+      </c>
+      <c r="B25" s="7">
+        <v>0.42611285261431397</v>
+      </c>
+      <c r="C25" s="7">
+        <v>0.45277101716294699</v>
+      </c>
+      <c r="D25">
+        <v>0.46960966995350401</v>
+      </c>
+      <c r="E25" s="7">
+        <v>0.50105902268361702</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="7">
+        <v>17</v>
+      </c>
+      <c r="B26" s="7">
+        <v>0.42688246462634899</v>
+      </c>
+      <c r="C26" s="7">
+        <v>0.45139470905720303</v>
+      </c>
+      <c r="D26">
+        <v>0.47141518180715902</v>
+      </c>
+      <c r="E26" s="7">
+        <v>0.50082237207601199</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="7">
+        <v>18</v>
+      </c>
+      <c r="B27" s="7">
+        <v>0.42788661627768698</v>
+      </c>
+      <c r="C27" s="7">
+        <v>0.45253420980249298</v>
+      </c>
+      <c r="D27">
+        <v>0.471745678765773</v>
+      </c>
+      <c r="E27" s="7">
+        <v>0.49911267879642601</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="7">
+        <v>19</v>
+      </c>
+      <c r="B28" s="7">
+        <v>0.42859435539555901</v>
+      </c>
+      <c r="C28" s="7">
+        <v>0.452711957497622</v>
+      </c>
+      <c r="D28">
+        <v>0.47435304020555102</v>
+      </c>
+      <c r="E28" s="7">
+        <v>0.49973851056142699</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="7">
+        <v>20</v>
+      </c>
+      <c r="B29" s="7">
+        <v>0.42674959990081501</v>
+      </c>
+      <c r="C29" s="7">
+        <v>0.45304094033761599</v>
+      </c>
+      <c r="D29">
+        <v>0.47525896523388</v>
+      </c>
+      <c r="E29" s="7">
+        <v>0.50185622995266999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="7">
+        <v>21</v>
+      </c>
+      <c r="B30" s="7">
+        <v>0.42789267357517402</v>
+      </c>
+      <c r="C30" s="7">
+        <v>0.454153658845104</v>
+      </c>
+      <c r="D30">
+        <v>0.47488783807352702</v>
+      </c>
+      <c r="E30" s="7">
+        <v>0.501870216262015</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="7">
+        <v>22</v>
+      </c>
+      <c r="B31" s="7">
+        <v>0.42658623458348099</v>
+      </c>
+      <c r="C31" s="7">
+        <v>0.457030123818565</v>
+      </c>
+      <c r="D31">
+        <v>0.47455656195282597</v>
+      </c>
+      <c r="E31" s="7">
+        <v>0.50114247739387097</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="7">
+        <v>23</v>
+      </c>
+      <c r="B32" s="7">
+        <v>0.42752780295738502</v>
+      </c>
+      <c r="C32" s="7">
+        <v>0.45815744739179998</v>
+      </c>
+      <c r="D32">
+        <v>0.475186100335935</v>
+      </c>
+      <c r="E32" s="7">
+        <v>0.50313361764063702</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="7">
+        <v>24</v>
+      </c>
+      <c r="B33" s="7">
+        <v>0.42771234980212602</v>
+      </c>
+      <c r="C33" s="7">
+        <v>0.45732264107385501</v>
+      </c>
+      <c r="D33">
+        <v>0.47520459656550501</v>
+      </c>
+      <c r="E33" s="7">
+        <v>0.50282887834676204</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="7">
+        <v>25</v>
+      </c>
+      <c r="B34" s="7">
+        <v>0.42564939725103901</v>
+      </c>
+      <c r="C34" s="7">
+        <v>0.45656920734150702</v>
+      </c>
+      <c r="D34">
+        <v>0.47471837581683901</v>
+      </c>
+      <c r="E34" s="7">
+        <v>0.50173612169128001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="7">
+        <v>26</v>
+      </c>
+      <c r="B35" s="7">
+        <v>0.42526094362174999</v>
+      </c>
+      <c r="C35" s="7">
+        <v>0.45586345820069502</v>
+      </c>
+      <c r="D35">
+        <v>0.47587054275225399</v>
+      </c>
+      <c r="E35" s="7">
+        <v>0.501522292936325</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="7">
+        <v>27</v>
+      </c>
+      <c r="B36" s="7">
+        <v>0.426246757103801</v>
+      </c>
+      <c r="C36" s="7">
+        <v>0.456792889563295</v>
+      </c>
+      <c r="D36">
+        <v>0.47645153627650499</v>
+      </c>
+      <c r="E36" s="7">
+        <v>0.50111257933980502</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="7">
+        <v>28</v>
+      </c>
+      <c r="B37" s="7">
+        <v>0.426615536590286</v>
+      </c>
+      <c r="C37" s="7">
+        <v>0.45776236992435398</v>
+      </c>
+      <c r="D37">
+        <v>0.476047379301481</v>
+      </c>
+      <c r="E37" s="7">
+        <v>0.50140426171459795</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="7">
+        <v>29</v>
+      </c>
+      <c r="B38" s="7">
+        <v>0.42764992296110599</v>
+      </c>
+      <c r="C38" s="7">
+        <v>0.45783340614117701</v>
+      </c>
+      <c r="D38">
+        <v>0.47644290783953902</v>
+      </c>
+      <c r="E38" s="7">
+        <v>0.50108045561947701</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="7">
+        <v>30</v>
+      </c>
+      <c r="B39" s="7">
+        <v>0.42933537131421001</v>
+      </c>
+      <c r="C39" s="7">
+        <v>0.458352593263265</v>
+      </c>
+      <c r="D39">
+        <v>0.47564473431758297</v>
+      </c>
+      <c r="E39" s="7">
+        <v>0.50060582681427201</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40" s="7">
+        <v>8989642</v>
+      </c>
+      <c r="C40" s="7">
+        <v>20692449</v>
+      </c>
+      <c r="D40">
+        <v>49221669</v>
+      </c>
+      <c r="E40" s="7">
+        <v>98042792</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>